<commit_message>
upd serpapi table + streamlit
</commit_message>
<xml_diff>
--- a/api_keys_status.xlsx
+++ b/api_keys_status.xlsx
@@ -526,7 +526,7 @@
         <v>447375313752</v>
       </c>
       <c r="E4" t="n">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5">
@@ -779,7 +779,7 @@
         <v>447399415357</v>
       </c>
       <c r="E15" t="n">
-        <v>100</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16">
@@ -917,7 +917,7 @@
         <v>447951289910</v>
       </c>
       <c r="E21" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reduction done need check
</commit_message>
<xml_diff>
--- a/api_keys_status.xlsx
+++ b/api_keys_status.xlsx
@@ -503,7 +503,7 @@
         <v>447415262566</v>
       </c>
       <c r="E3" t="n">
-        <v>98</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -526,7 +526,7 @@
         <v>447375313752</v>
       </c>
       <c r="E4" t="n">
-        <v>96</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -549,7 +549,7 @@
         <v>447719427866</v>
       </c>
       <c r="E5" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -572,7 +572,7 @@
         <v>447351831178</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -595,7 +595,7 @@
         <v>447958450698</v>
       </c>
       <c r="E7" t="n">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
@@ -618,7 +618,7 @@
         <v>447386761934</v>
       </c>
       <c r="E8" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
@@ -641,7 +641,7 @@
         <v>447448025599</v>
       </c>
       <c r="E9" t="n">
-        <v>100</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -664,7 +664,7 @@
         <v>447448346445</v>
       </c>
       <c r="E10" t="n">
-        <v>100</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
@@ -710,7 +710,7 @@
         <v>447459939078</v>
       </c>
       <c r="E12" t="n">
-        <v>100</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
@@ -733,7 +733,7 @@
         <v>447398744361</v>
       </c>
       <c r="E13" t="n">
-        <v>100</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
@@ -779,7 +779,7 @@
         <v>447399415357</v>
       </c>
       <c r="E15" t="n">
-        <v>44</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -825,7 +825,7 @@
         <v>447405706428</v>
       </c>
       <c r="E17" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -917,7 +917,7 @@
         <v>447951289910</v>
       </c>
       <c r="E21" t="n">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tone of voice prompt upd
</commit_message>
<xml_diff>
--- a/api_keys_status.xlsx
+++ b/api_keys_status.xlsx
@@ -503,7 +503,7 @@
         <v>447415262566</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -526,7 +526,7 @@
         <v>447375313752</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -641,7 +641,7 @@
         <v>447448025599</v>
       </c>
       <c r="E9" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -779,7 +779,7 @@
         <v>447399415357</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
trying to parse avia and book data
</commit_message>
<xml_diff>
--- a/api_keys_status.xlsx
+++ b/api_keys_status.xlsx
@@ -503,7 +503,7 @@
         <v>447415262566</v>
       </c>
       <c r="E3" t="n">
-        <v>98</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -526,7 +526,7 @@
         <v>447375313752</v>
       </c>
       <c r="E4" t="n">
-        <v>96</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -549,7 +549,7 @@
         <v>447719427866</v>
       </c>
       <c r="E5" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -572,7 +572,7 @@
         <v>447351831178</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -595,7 +595,7 @@
         <v>447958450698</v>
       </c>
       <c r="E7" t="n">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -618,7 +618,7 @@
         <v>447386761934</v>
       </c>
       <c r="E8" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -641,7 +641,7 @@
         <v>447448025599</v>
       </c>
       <c r="E9" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -664,7 +664,7 @@
         <v>447448346445</v>
       </c>
       <c r="E10" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -710,7 +710,7 @@
         <v>447459939078</v>
       </c>
       <c r="E12" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
@@ -733,7 +733,7 @@
         <v>447398744361</v>
       </c>
       <c r="E13" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -779,7 +779,7 @@
         <v>447399415357</v>
       </c>
       <c r="E15" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -825,7 +825,7 @@
         <v>447405706428</v>
       </c>
       <c r="E17" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -917,7 +917,7 @@
         <v>447951289910</v>
       </c>
       <c r="E21" t="n">
-        <v>55</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: implement offer generation service from vtbfamily
</commit_message>
<xml_diff>
--- a/api_keys_status.xlsx
+++ b/api_keys_status.xlsx
@@ -710,7 +710,7 @@
         <v>447459939078</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -779,7 +779,7 @@
         <v>447399415357</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -917,7 +917,7 @@
         <v>447951289910</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -940,7 +940,7 @@
         <v>447951289910</v>
       </c>
       <c r="E22" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
@@ -963,7 +963,7 @@
         <v>11111</v>
       </c>
       <c r="E23" t="n">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24">
@@ -986,7 +986,7 @@
         <v>11111</v>
       </c>
       <c r="E24" t="n">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25">
@@ -1009,7 +1009,7 @@
         <v>11111</v>
       </c>
       <c r="E25" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26">
@@ -1032,7 +1032,7 @@
         <v>11111</v>
       </c>
       <c r="E26" t="n">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: update serp api keys table
</commit_message>
<xml_diff>
--- a/api_keys_status.xlsx
+++ b/api_keys_status.xlsx
@@ -710,7 +710,7 @@
         <v>447459939078</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -779,7 +779,7 @@
         <v>447399415357</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -917,7 +917,7 @@
         <v>447951289910</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -940,7 +940,7 @@
         <v>447951289910</v>
       </c>
       <c r="E22" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23">
@@ -963,7 +963,7 @@
         <v>11111</v>
       </c>
       <c r="E23" t="n">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24">
@@ -986,7 +986,7 @@
         <v>11111</v>
       </c>
       <c r="E24" t="n">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25">
@@ -1009,7 +1009,7 @@
         <v>11111</v>
       </c>
       <c r="E25" t="n">
-        <v>16</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26">
@@ -1032,7 +1032,7 @@
         <v>11111</v>
       </c>
       <c r="E26" t="n">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: chroma compatibility with sqlite and system prompt for offersgen
</commit_message>
<xml_diff>
--- a/api_keys_status.xlsx
+++ b/api_keys_status.xlsx
@@ -710,7 +710,7 @@
         <v>447459939078</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -779,7 +779,7 @@
         <v>447399415357</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -917,7 +917,7 @@
         <v>447951289910</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -940,7 +940,7 @@
         <v>447951289910</v>
       </c>
       <c r="E22" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
@@ -963,7 +963,7 @@
         <v>11111</v>
       </c>
       <c r="E23" t="n">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24">
@@ -986,7 +986,7 @@
         <v>11111</v>
       </c>
       <c r="E24" t="n">
-        <v>46</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
@@ -1009,7 +1009,7 @@
         <v>11111</v>
       </c>
       <c r="E25" t="n">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
@@ -1032,7 +1032,7 @@
         <v>11111</v>
       </c>
       <c r="E26" t="n">
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>